<commit_message>
Add Some Missing Prompts
</commit_message>
<xml_diff>
--- a/Prompts/Pizza Shop IVR.xlsx
+++ b/Prompts/Pizza Shop IVR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IST\Moaz\Work\Training\internship-material\Prompts\Matrices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IST\Moaz\Work\Training\internship-material\Prompts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8859F7-372C-4E97-9078-B493B949A853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2D91F8-A23D-4AF0-81EE-6852F50FCE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Filename</t>
   </si>
@@ -119,15 +119,40 @@
   </si>
   <si>
     <t>للتحدث مع أحد موظفي خدمة العملاء، اضغط 1. لطلب بيتزا، اضغط 2. لتتبع طلبك، اضغط 3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxTries.wav </t>
+  </si>
+  <si>
+    <t>Sorry, you have exceeded the maximum number of attempts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عذراً، لقد تجاوزت الحد الأقصى لعدد المحاولات. </t>
+  </si>
+  <si>
+    <t>LangMenu.wav</t>
+  </si>
+  <si>
+    <t>For English press 2</t>
+  </si>
+  <si>
+    <t>للغة العربية اضغط 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -154,13 +179,85 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -174,12 +271,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0">
-  <autoFilter ref="A1:C11" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}" name="Table1" displayName="Table1" ref="A1:C13" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0">
+  <autoFilter ref="A1:C13" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{431E7D01-4C8C-45A7-9890-7F9DAB5E3FF8}" name="Filename"/>
-    <tableColumn id="2" xr3:uid="{6A61AEBB-1DDD-4534-B106-0317F365822A}" name="English Prompt"/>
-    <tableColumn id="3" xr3:uid="{10FE843A-FA84-419C-BDEC-1CB364B8B8E4}" name="Arabic Prompt"/>
+    <tableColumn id="1" xr3:uid="{431E7D01-4C8C-45A7-9890-7F9DAB5E3FF8}" name="Filename" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{6A61AEBB-1DDD-4534-B106-0317F365822A}" name="English Prompt" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{10FE843A-FA84-419C-BDEC-1CB364B8B8E4}" name="Arabic Prompt" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -507,137 +604,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Integrate Pizza IVR With API
</commit_message>
<xml_diff>
--- a/Prompts/Pizza Shop IVR.xlsx
+++ b/Prompts/Pizza Shop IVR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IST\Moaz\Work\Training\internship-material\Prompts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2D91F8-A23D-4AF0-81EE-6852F50FCE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8510BC42-C2BB-4852-A699-F192BC34D70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Filename</t>
   </si>
@@ -61,15 +61,6 @@
     <t>عذراً، هذا خيار غير صحيح.</t>
   </si>
   <si>
-    <t>OrderConfirmed.wav</t>
-  </si>
-  <si>
-    <t>Your order will be ready in 20 minutes.</t>
-  </si>
-  <si>
-    <t>طلبك سيكون جاهزاً خلال 20 دقيقة.</t>
-  </si>
-  <si>
     <t>ShopClosed.wav</t>
   </si>
   <si>
@@ -137,15 +128,58 @@
   </si>
   <si>
     <t>للغة العربية اضغط 1</t>
+  </si>
+  <si>
+    <t>OrderDelivered.wav</t>
+  </si>
+  <si>
+    <t>Your order has been delivered.</t>
+  </si>
+  <si>
+    <t>تم توصيل طلبك.</t>
+  </si>
+  <si>
+    <t>OrderCreated.wav</t>
+  </si>
+  <si>
+    <t>Your order has been created with number</t>
+  </si>
+  <si>
+    <t>تم إنشاء طلبك بالرقم</t>
+  </si>
+  <si>
+    <t>WillBeReadyIn.wav</t>
+  </si>
+  <si>
+    <t>It will be ready in</t>
+  </si>
+  <si>
+    <t>سيكون جاهزاً خلال</t>
+  </si>
+  <si>
+    <t>Minutes.wav</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>دقائق</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -179,8 +213,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -271,12 +309,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}" name="Table1" displayName="Table1" ref="A1:C13" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0">
-  <autoFilter ref="A1:C13" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C16" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{431E7D01-4C8C-45A7-9890-7F9DAB5E3FF8}" name="Filename" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{6A61AEBB-1DDD-4534-B106-0317F365822A}" name="English Prompt" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{10FE843A-FA84-419C-BDEC-1CB364B8B8E4}" name="Arabic Prompt" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{431E7D01-4C8C-45A7-9890-7F9DAB5E3FF8}" name="Filename" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{6A61AEBB-1DDD-4534-B106-0317F365822A}" name="English Prompt" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{10FE843A-FA84-419C-BDEC-1CB364B8B8E4}" name="Arabic Prompt" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -604,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,13 +680,13 @@
     </row>
     <row r="3" spans="1:3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -656,10 +694,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -686,79 +724,112 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
+      <c r="A12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
+      <c r="A13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>